<commit_message>
fix feedback no.3, 8, 24, 30, 31
</commit_message>
<xml_diff>
--- a/rtw_excel_report/report_purchase_order_for_part/purchase_order_for_part.xlsx
+++ b/rtw_excel_report/report_purchase_order_for_part/purchase_order_for_part.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\odoo\rtw-custom\rtw_excel_report\report_purchase_order_for_part\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74E48D-C699-4FC1-A469-DFD241C1B723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC8D8FB-0C3E-4D55-91EA-E8ED7C08D665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02D0CE77-5587-4803-AB74-D622CD74C233}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02D0CE77-5587-4803-AB74-D622CD74C233}"/>
   </bookViews>
   <sheets>
     <sheet name="発注書(部材用）" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,10 @@
     <t>発注金額合計</t>
   </si>
   <si>
-    <t>Config</t>
+    <t>備送り先注記:</t>
   </si>
   <si>
-    <t>備送り先注記:</t>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -789,7 +789,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="15"/>
       <c r="G10" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -871,7 +871,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>